<commit_message>
Linked List: Middle of the Linked List
</commit_message>
<xml_diff>
--- a/#DSASheetbyArsh (45-60 Days).xlsx
+++ b/#DSASheetbyArsh (45-60 Days).xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kunal\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kunal\OneDrive\Desktop\vs code\45DaysDSAChallenge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83B31490-D955-4A53-89CB-B5FF85990592}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{338E50F9-9703-40DB-95C7-4C57988EDBAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4044" yWindow="3276" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="794" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="795" uniqueCount="324">
   <si>
     <t>#CrackYourInternship</t>
   </si>
@@ -1491,8 +1491,8 @@
   </sheetPr>
   <dimension ref="A1:I333"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A119" workbookViewId="0">
-      <selection activeCell="D129" sqref="D129"/>
+    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
+      <selection activeCell="C97" sqref="C97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -2379,6 +2379,9 @@
       </c>
       <c r="C97" s="9" t="s">
         <v>98</v>
+      </c>
+      <c r="D97" t="s">
+        <v>323</v>
       </c>
     </row>
     <row r="98" spans="2:9" ht="13.2">
@@ -4883,5 +4886,6 @@
     <hyperlink ref="C133" r:id="rId300" xr:uid="{00000000-0004-0000-0000-000073000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId301"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update DSASheetbyArsh (45-60 Days).xlsx
</commit_message>
<xml_diff>
--- a/#DSASheetbyArsh (45-60 Days).xlsx
+++ b/#DSASheetbyArsh (45-60 Days).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kunal\OneDrive\Desktop\vs code\45DaysDSAChallenge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43D481B0-E846-46BB-BF35-167686096059}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE170BEA-F530-4808-85AD-15C8C7F9A588}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="804" uniqueCount="327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="805" uniqueCount="328">
   <si>
     <t>#CrackYourInternship</t>
   </si>
@@ -1033,6 +1033,9 @@
   </si>
   <si>
     <t>Done(7/07/23)</t>
+  </si>
+  <si>
+    <t>Done(8/7/23)</t>
   </si>
 </sst>
 </file>
@@ -1500,8 +1503,8 @@
   </sheetPr>
   <dimension ref="A1:I333"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="70" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" zoomScale="70" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -1643,6 +1646,9 @@
       </c>
       <c r="C13" s="9" t="s">
         <v>20</v>
+      </c>
+      <c r="D13" t="s">
+        <v>327</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="13.2">

</xml_diff>

<commit_message>
Array: (18)Choclate Distribution Problem.cpp
</commit_message>
<xml_diff>
--- a/#DSASheetbyArsh (45-60 Days).xlsx
+++ b/#DSASheetbyArsh (45-60 Days).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kunal\OneDrive\Desktop\vs code\45DaysDSAChallenge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE170BEA-F530-4808-85AD-15C8C7F9A588}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E113F097-20E1-4E5A-8A20-6DF093CCB62A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="805" uniqueCount="328">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="806" uniqueCount="328">
   <si>
     <t>#CrackYourInternship</t>
   </si>
@@ -1504,7 +1504,7 @@
   <dimension ref="A1:I333"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -1606,6 +1606,9 @@
       </c>
       <c r="C9" s="9" t="s">
         <v>16</v>
+      </c>
+      <c r="D9" t="s">
+        <v>327</v>
       </c>
       <c r="E9" s="11"/>
     </row>

</xml_diff>

<commit_message>
Graph: BFS of Graph
</commit_message>
<xml_diff>
--- a/#DSASheetbyArsh (45-60 Days).xlsx
+++ b/#DSASheetbyArsh (45-60 Days).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kunal\OneDrive\Desktop\vs code\45DaysDSAChallenge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E113F097-20E1-4E5A-8A20-6DF093CCB62A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F81DEF9-143A-4CC1-B82A-7C3A78270C3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="806" uniqueCount="328">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="807" uniqueCount="329">
   <si>
     <t>#CrackYourInternship</t>
   </si>
@@ -1036,6 +1036,9 @@
   </si>
   <si>
     <t>Done(8/7/23)</t>
+  </si>
+  <si>
+    <t>Done(10/07/23)</t>
   </si>
 </sst>
 </file>
@@ -1503,8 +1506,8 @@
   </sheetPr>
   <dimension ref="A1:I333"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="A187" zoomScale="58" workbookViewId="0">
+      <selection activeCell="C194" sqref="C194"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -3365,6 +3368,9 @@
       </c>
       <c r="C194" s="9" t="s">
         <v>192</v>
+      </c>
+      <c r="D194" t="s">
+        <v>328</v>
       </c>
       <c r="G194" s="11" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Graph: DFS of Graph
</commit_message>
<xml_diff>
--- a/#DSASheetbyArsh (45-60 Days).xlsx
+++ b/#DSASheetbyArsh (45-60 Days).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kunal\OneDrive\Desktop\vs code\45DaysDSAChallenge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F81DEF9-143A-4CC1-B82A-7C3A78270C3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3512F1A2-11D8-4B07-B0C5-03CAF1D7B1DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="807" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="808" uniqueCount="329">
   <si>
     <t>#CrackYourInternship</t>
   </si>
@@ -1506,8 +1506,8 @@
   </sheetPr>
   <dimension ref="A1:I333"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A187" zoomScale="58" workbookViewId="0">
-      <selection activeCell="C194" sqref="C194"/>
+    <sheetView tabSelected="1" topLeftCell="B190" zoomScale="87" workbookViewId="0">
+      <selection activeCell="E195" sqref="E195"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -3382,6 +3382,9 @@
       </c>
       <c r="C195" s="9" t="s">
         <v>193</v>
+      </c>
+      <c r="D195" t="s">
+        <v>328</v>
       </c>
       <c r="E195" s="11" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Graph: (20)No. of Provinces.cpp
</commit_message>
<xml_diff>
--- a/#DSASheetbyArsh (45-60 Days).xlsx
+++ b/#DSASheetbyArsh (45-60 Days).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kunal\OneDrive\Desktop\vs code\45DaysDSAChallenge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3512F1A2-11D8-4B07-B0C5-03CAF1D7B1DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3924438D-AFDA-464B-AFEC-72C6F1D6300E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="808" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="811" uniqueCount="331">
   <si>
     <t>#CrackYourInternship</t>
   </si>
@@ -1039,6 +1039,12 @@
   </si>
   <si>
     <t>Done(10/07/23)</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/number-of-provinces/description/</t>
+  </si>
+  <si>
+    <t>Done(11/07/23)</t>
   </si>
 </sst>
 </file>
@@ -1504,10 +1510,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:I333"/>
+  <dimension ref="A1:I334"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B190" zoomScale="87" workbookViewId="0">
-      <selection activeCell="E195" sqref="E195"/>
+    <sheetView tabSelected="1" topLeftCell="B204" zoomScale="87" workbookViewId="0">
+      <selection activeCell="C215" sqref="C215"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -3571,7 +3577,10 @@
         <v>22</v>
       </c>
       <c r="C215" s="9" t="s">
-        <v>213</v>
+        <v>329</v>
+      </c>
+      <c r="D215" t="s">
+        <v>330</v>
       </c>
     </row>
     <row r="216" spans="2:9" ht="13.2">
@@ -3579,7 +3588,7 @@
         <v>22</v>
       </c>
       <c r="C216" s="9" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="217" spans="2:9" ht="13.2">
@@ -3587,10 +3596,7 @@
         <v>22</v>
       </c>
       <c r="C217" s="9" t="s">
-        <v>215</v>
-      </c>
-      <c r="I217" s="11" t="s">
-        <v>13</v>
+        <v>214</v>
       </c>
     </row>
     <row r="218" spans="2:9" ht="13.2">
@@ -3598,12 +3604,9 @@
         <v>22</v>
       </c>
       <c r="C218" s="9" t="s">
-        <v>216</v>
-      </c>
-      <c r="F218" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="H218" s="11" t="s">
+        <v>215</v>
+      </c>
+      <c r="I218" s="11" t="s">
         <v>13</v>
       </c>
     </row>
@@ -3612,7 +3615,13 @@
         <v>22</v>
       </c>
       <c r="C219" s="9" t="s">
-        <v>217</v>
+        <v>216</v>
+      </c>
+      <c r="F219" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="H219" s="11" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="220" spans="2:9" ht="13.2">
@@ -3620,18 +3629,15 @@
         <v>22</v>
       </c>
       <c r="C220" s="9" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="221" spans="2:9" ht="13.2">
       <c r="B221" s="8" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="C221" s="9" t="s">
-        <v>219</v>
-      </c>
-      <c r="E221" s="11" t="s">
-        <v>13</v>
+        <v>218</v>
       </c>
     </row>
     <row r="222" spans="2:9" ht="13.2">
@@ -3639,7 +3645,10 @@
         <v>38</v>
       </c>
       <c r="C222" s="9" t="s">
-        <v>220</v>
+        <v>219</v>
+      </c>
+      <c r="E222" s="11" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="223" spans="2:9" ht="13.2">
@@ -3647,13 +3656,7 @@
         <v>38</v>
       </c>
       <c r="C223" s="9" t="s">
-        <v>221</v>
-      </c>
-      <c r="H223" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="I223" s="11" t="s">
-        <v>13</v>
+        <v>220</v>
       </c>
     </row>
     <row r="224" spans="2:9" ht="13.2">
@@ -3661,9 +3664,12 @@
         <v>38</v>
       </c>
       <c r="C224" s="9" t="s">
-        <v>222</v>
-      </c>
-      <c r="G224" s="11" t="s">
+        <v>221</v>
+      </c>
+      <c r="H224" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="I224" s="11" t="s">
         <v>13</v>
       </c>
     </row>
@@ -3672,13 +3678,10 @@
         <v>38</v>
       </c>
       <c r="C225" s="9" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G225" s="11" t="s">
         <v>13</v>
-      </c>
-      <c r="I225" s="5" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="226" spans="2:9" ht="13.2">
@@ -3686,33 +3689,39 @@
         <v>38</v>
       </c>
       <c r="C226" s="9" t="s">
-        <v>225</v>
-      </c>
-      <c r="G226" s="11"/>
+        <v>223</v>
+      </c>
+      <c r="G226" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="I226" s="5" t="s">
+        <v>224</v>
+      </c>
     </row>
     <row r="227" spans="2:9" ht="13.2">
       <c r="B227" s="8" t="s">
         <v>38</v>
       </c>
       <c r="C227" s="9" t="s">
-        <v>226</v>
-      </c>
-      <c r="G227" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="H227" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="I227" s="11" t="s">
-        <v>13</v>
-      </c>
+        <v>225</v>
+      </c>
+      <c r="G227" s="11"/>
     </row>
     <row r="228" spans="2:9" ht="13.2">
       <c r="B228" s="8" t="s">
         <v>38</v>
       </c>
       <c r="C228" s="9" t="s">
-        <v>227</v>
+        <v>226</v>
+      </c>
+      <c r="G228" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="H228" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="I228" s="11" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="229" spans="2:9" ht="13.2">
@@ -3720,33 +3729,33 @@
         <v>38</v>
       </c>
       <c r="C229" s="9" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="230" spans="2:9" ht="13.2">
       <c r="B230" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C230" s="14" t="s">
+      <c r="C230" s="9" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="231" spans="2:9" ht="13.2">
+      <c r="B231" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C231" s="14" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="231" spans="2:9" ht="13.2">
-      <c r="B231" s="6"/>
-      <c r="C231" s="6"/>
     </row>
     <row r="232" spans="2:9" ht="13.2">
       <c r="B232" s="6"/>
-      <c r="C232" s="24" t="s">
+      <c r="C232" s="6"/>
+    </row>
+    <row r="233" spans="2:9" ht="13.2">
+      <c r="B233" s="6"/>
+      <c r="C233" s="24" t="s">
         <v>230</v>
-      </c>
-    </row>
-    <row r="233" spans="2:9" ht="13.2">
-      <c r="B233" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C233" s="9" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="234" spans="2:9" ht="13.2">
@@ -3754,10 +3763,7 @@
         <v>22</v>
       </c>
       <c r="C234" s="9" t="s">
-        <v>232</v>
-      </c>
-      <c r="E234" s="11" t="s">
-        <v>13</v>
+        <v>231</v>
       </c>
     </row>
     <row r="235" spans="2:9" ht="13.2">
@@ -3765,7 +3771,7 @@
         <v>22</v>
       </c>
       <c r="C235" s="9" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E235" s="11" t="s">
         <v>13</v>
@@ -3776,7 +3782,7 @@
         <v>22</v>
       </c>
       <c r="C236" s="9" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E236" s="11" t="s">
         <v>13</v>
@@ -3784,10 +3790,10 @@
     </row>
     <row r="237" spans="2:9" ht="13.2">
       <c r="B237" s="8" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="C237" s="9" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E237" s="11" t="s">
         <v>13</v>
@@ -3798,37 +3804,40 @@
         <v>38</v>
       </c>
       <c r="C238" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="E238" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="239" spans="2:9" ht="13.2">
+      <c r="B239" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C239" s="9" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="239" spans="2:9" ht="13.2">
-      <c r="B239" s="6"/>
-      <c r="C239" s="6"/>
     </row>
     <row r="240" spans="2:9" ht="13.2">
       <c r="B240" s="6"/>
-      <c r="C240" s="20" t="s">
-        <v>237</v>
-      </c>
+      <c r="C240" s="6"/>
     </row>
     <row r="241" spans="2:7" ht="13.2">
       <c r="B241" s="6"/>
-      <c r="C241" s="6"/>
+      <c r="C241" s="20" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="242" spans="2:7" ht="13.2">
-      <c r="B242" s="8" t="s">
-        <v>238</v>
-      </c>
-      <c r="C242" s="9" t="s">
-        <v>239</v>
-      </c>
+      <c r="B242" s="6"/>
+      <c r="C242" s="6"/>
     </row>
     <row r="243" spans="2:7" ht="13.2">
       <c r="B243" s="8" t="s">
         <v>238</v>
       </c>
-      <c r="C243" s="3" t="s">
-        <v>240</v>
+      <c r="C243" s="9" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="244" spans="2:7" ht="13.2">
@@ -3836,7 +3845,7 @@
         <v>238</v>
       </c>
       <c r="C244" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="245" spans="2:7" ht="13.2">
@@ -3844,7 +3853,7 @@
         <v>238</v>
       </c>
       <c r="C245" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="246" spans="2:7" ht="13.2">
@@ -3852,7 +3861,7 @@
         <v>238</v>
       </c>
       <c r="C246" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="247" spans="2:7" ht="13.2">
@@ -3860,7 +3869,7 @@
         <v>238</v>
       </c>
       <c r="C247" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="248" spans="2:7" ht="13.2">
@@ -3868,42 +3877,42 @@
         <v>238</v>
       </c>
       <c r="C248" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="249" spans="2:7" ht="13.2">
       <c r="B249" s="8" t="s">
         <v>238</v>
       </c>
-      <c r="C249" s="14" t="s">
-        <v>246</v>
+      <c r="C249" s="3" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="250" spans="2:7" ht="13.2">
       <c r="B250" s="8" t="s">
         <v>238</v>
       </c>
-      <c r="C250" s="9" t="s">
-        <v>247</v>
-      </c>
-      <c r="G250" s="11" t="s">
-        <v>13</v>
+      <c r="C250" s="14" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="251" spans="2:7" ht="13.2">
       <c r="B251" s="8" t="s">
         <v>238</v>
       </c>
-      <c r="C251" s="3" t="s">
-        <v>248</v>
+      <c r="C251" s="9" t="s">
+        <v>247</v>
+      </c>
+      <c r="G251" s="11" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="252" spans="2:7" ht="13.2">
       <c r="B252" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="C252" s="9" t="s">
-        <v>249</v>
+        <v>238</v>
+      </c>
+      <c r="C252" s="3" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="253" spans="2:7" ht="13.2">
@@ -3911,10 +3920,7 @@
         <v>38</v>
       </c>
       <c r="C253" s="9" t="s">
-        <v>250</v>
-      </c>
-      <c r="E253" s="11" t="s">
-        <v>13</v>
+        <v>249</v>
       </c>
     </row>
     <row r="254" spans="2:7" ht="13.2">
@@ -3922,7 +3928,10 @@
         <v>38</v>
       </c>
       <c r="C254" s="9" t="s">
-        <v>251</v>
+        <v>250</v>
+      </c>
+      <c r="E254" s="11" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="255" spans="2:7" ht="13.2">
@@ -3930,25 +3939,25 @@
         <v>38</v>
       </c>
       <c r="C255" s="9" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="256" spans="2:7" ht="13.2">
+      <c r="B256" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C256" s="9" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="256" spans="2:7" ht="13.2">
-      <c r="B256" s="6"/>
-      <c r="C256" s="6"/>
     </row>
     <row r="257" spans="2:9" ht="13.2">
       <c r="B257" s="6"/>
-      <c r="C257" s="24" t="s">
+      <c r="C257" s="6"/>
+    </row>
+    <row r="258" spans="2:9" ht="13.2">
+      <c r="B258" s="6"/>
+      <c r="C258" s="24" t="s">
         <v>253</v>
-      </c>
-    </row>
-    <row r="258" spans="2:9" ht="13.2">
-      <c r="B258" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C258" s="9" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="259" spans="2:9" ht="13.2">
@@ -3956,10 +3965,7 @@
         <v>11</v>
       </c>
       <c r="C259" s="9" t="s">
-        <v>255</v>
-      </c>
-      <c r="F259" s="11" t="s">
-        <v>13</v>
+        <v>254</v>
       </c>
     </row>
     <row r="260" spans="2:9" ht="13.2">
@@ -3967,9 +3973,9 @@
         <v>11</v>
       </c>
       <c r="C260" s="9" t="s">
-        <v>256</v>
-      </c>
-      <c r="I260" s="11" t="s">
+        <v>255</v>
+      </c>
+      <c r="F260" s="11" t="s">
         <v>13</v>
       </c>
     </row>
@@ -3978,45 +3984,45 @@
         <v>11</v>
       </c>
       <c r="C261" s="9" t="s">
-        <v>257</v>
-      </c>
-      <c r="H261" s="11" t="s">
+        <v>256</v>
+      </c>
+      <c r="I261" s="11" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="262" spans="2:9" ht="13.2">
       <c r="B262" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C262" s="3" t="s">
-        <v>258</v>
+        <v>11</v>
+      </c>
+      <c r="C262" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="H262" s="11" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="263" spans="2:9" ht="13.2">
       <c r="B263" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C263" s="9" t="s">
-        <v>259</v>
+      <c r="C263" s="3" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="264" spans="2:9" ht="13.2">
       <c r="B264" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C264" s="3" t="s">
-        <v>260</v>
-      </c>
-      <c r="E264" s="11" t="s">
-        <v>13</v>
+      <c r="C264" s="9" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="265" spans="2:9" ht="13.2">
       <c r="B265" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C265" s="9" t="s">
-        <v>261</v>
+      <c r="C265" s="3" t="s">
+        <v>260</v>
       </c>
       <c r="E265" s="11" t="s">
         <v>13</v>
@@ -4027,10 +4033,9 @@
         <v>22</v>
       </c>
       <c r="C266" s="9" t="s">
-        <v>262</v>
-      </c>
-      <c r="E266" s="11"/>
-      <c r="I266" s="11" t="s">
+        <v>261</v>
+      </c>
+      <c r="E266" s="11" t="s">
         <v>13</v>
       </c>
     </row>
@@ -4039,12 +4044,10 @@
         <v>22</v>
       </c>
       <c r="C267" s="9" t="s">
-        <v>263</v>
-      </c>
-      <c r="E267" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="H267" s="11" t="s">
+        <v>262</v>
+      </c>
+      <c r="E267" s="11"/>
+      <c r="I267" s="11" t="s">
         <v>13</v>
       </c>
     </row>
@@ -4053,7 +4056,10 @@
         <v>22</v>
       </c>
       <c r="C268" s="9" t="s">
-        <v>264</v>
+        <v>263</v>
+      </c>
+      <c r="E268" s="11" t="s">
+        <v>13</v>
       </c>
       <c r="H268" s="11" t="s">
         <v>13</v>
@@ -4063,30 +4069,30 @@
       <c r="B269" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C269" s="3" t="s">
-        <v>265</v>
-      </c>
-      <c r="H269" s="11"/>
+      <c r="C269" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="H269" s="11" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="270" spans="2:9" ht="13.2">
       <c r="B270" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C270" s="9" t="s">
-        <v>266</v>
-      </c>
-      <c r="H270" s="11" t="s">
-        <v>13</v>
-      </c>
+      <c r="C270" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="H270" s="11"/>
     </row>
     <row r="271" spans="2:9" ht="13.2">
       <c r="B271" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C271" s="3" t="s">
-        <v>267</v>
-      </c>
-      <c r="F271" s="11" t="s">
+      <c r="C271" s="9" t="s">
+        <v>266</v>
+      </c>
+      <c r="H271" s="11" t="s">
         <v>13</v>
       </c>
     </row>
@@ -4094,8 +4100,11 @@
       <c r="B272" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C272" s="9" t="s">
-        <v>268</v>
+      <c r="C272" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="F272" s="11" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="273" spans="2:9" ht="13.2">
@@ -4103,7 +4112,7 @@
         <v>22</v>
       </c>
       <c r="C273" s="9" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="274" spans="2:9" ht="13.2">
@@ -4111,7 +4120,7 @@
         <v>22</v>
       </c>
       <c r="C274" s="9" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="275" spans="2:9" ht="13.2">
@@ -4119,34 +4128,34 @@
         <v>22</v>
       </c>
       <c r="C275" s="9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="276" spans="2:9" ht="13.2">
       <c r="B276" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C276" s="3" t="s">
-        <v>272</v>
-      </c>
-      <c r="H276" s="11" t="s">
-        <v>13</v>
+      <c r="C276" s="9" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="277" spans="2:9" ht="13.2">
       <c r="B277" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="C277" s="9" t="s">
-        <v>273</v>
+        <v>22</v>
+      </c>
+      <c r="C277" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="H277" s="11" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="278" spans="2:9" ht="13.2">
       <c r="B278" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C278" s="3" t="s">
-        <v>274</v>
+      <c r="C278" s="9" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="279" spans="2:9" ht="13.2">
@@ -4154,10 +4163,7 @@
         <v>38</v>
       </c>
       <c r="C279" s="3" t="s">
-        <v>275</v>
-      </c>
-      <c r="F279" s="11" t="s">
-        <v>13</v>
+        <v>274</v>
       </c>
     </row>
     <row r="280" spans="2:9" ht="13.2">
@@ -4165,18 +4171,18 @@
         <v>38</v>
       </c>
       <c r="C280" s="3" t="s">
-        <v>276</v>
+        <v>275</v>
+      </c>
+      <c r="F280" s="11" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="281" spans="2:9" ht="13.2">
       <c r="B281" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C281" s="9" t="s">
-        <v>277</v>
-      </c>
-      <c r="I281" s="11" t="s">
-        <v>13</v>
+      <c r="C281" s="3" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="282" spans="2:9" ht="13.2">
@@ -4184,12 +4190,9 @@
         <v>38</v>
       </c>
       <c r="C282" s="9" t="s">
-        <v>278</v>
-      </c>
-      <c r="D282" t="s">
-        <v>323</v>
-      </c>
-      <c r="E282" s="11" t="s">
+        <v>277</v>
+      </c>
+      <c r="I282" s="11" t="s">
         <v>13</v>
       </c>
     </row>
@@ -4197,8 +4200,11 @@
       <c r="B283" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C283" s="3" t="s">
-        <v>279</v>
+      <c r="C283" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="D283" t="s">
+        <v>323</v>
       </c>
       <c r="E283" s="11" t="s">
         <v>13</v>
@@ -4209,7 +4215,7 @@
         <v>38</v>
       </c>
       <c r="C284" s="3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E284" s="11" t="s">
         <v>13</v>
@@ -4219,8 +4225,8 @@
       <c r="B285" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C285" s="9" t="s">
-        <v>281</v>
+      <c r="C285" s="3" t="s">
+        <v>280</v>
       </c>
       <c r="E285" s="11" t="s">
         <v>13</v>
@@ -4230,8 +4236,11 @@
       <c r="B286" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C286" s="3" t="s">
-        <v>282</v>
+      <c r="C286" s="9" t="s">
+        <v>281</v>
+      </c>
+      <c r="E286" s="11" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="287" spans="2:9" ht="13.2">
@@ -4239,31 +4248,28 @@
         <v>38</v>
       </c>
       <c r="C287" s="3" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="288" spans="2:9" ht="13.2">
+      <c r="B288" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C288" s="3" t="s">
         <v>283</v>
-      </c>
-    </row>
-    <row r="288" spans="2:9" ht="13.2">
-      <c r="B288" s="6"/>
-      <c r="C288" s="6"/>
-      <c r="I288" s="11" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="289" spans="2:9" ht="13.2">
       <c r="B289" s="6"/>
-      <c r="C289" s="3" t="s">
+      <c r="C289" s="6"/>
+      <c r="I289" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="290" spans="2:9" ht="13.2">
+      <c r="B290" s="6"/>
+      <c r="C290" s="3" t="s">
         <v>284</v>
-      </c>
-    </row>
-    <row r="290" spans="2:9" ht="13.2">
-      <c r="B290" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C290" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H290" s="11" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="291" spans="2:9" ht="13.2">
@@ -4271,7 +4277,10 @@
         <v>22</v>
       </c>
       <c r="C291" s="3" t="s">
-        <v>285</v>
+        <v>18</v>
+      </c>
+      <c r="H291" s="11" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="292" spans="2:9" ht="13.2">
@@ -4279,12 +4288,16 @@
         <v>22</v>
       </c>
       <c r="C292" s="3" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="293" spans="2:9" ht="13.2">
+      <c r="B293" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C293" s="3" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="293" spans="2:9" ht="13.2">
-      <c r="B293" s="6"/>
-      <c r="C293" s="6"/>
     </row>
     <row r="294" spans="2:9" ht="13.2">
       <c r="B294" s="6"/>
@@ -4292,35 +4305,28 @@
     </row>
     <row r="295" spans="2:9" ht="13.2">
       <c r="B295" s="6"/>
-      <c r="C295" s="3" t="s">
+      <c r="C295" s="6"/>
+    </row>
+    <row r="296" spans="2:9" ht="13.2">
+      <c r="B296" s="6"/>
+      <c r="C296" s="3" t="s">
         <v>287</v>
-      </c>
-    </row>
-    <row r="296" spans="2:9" ht="13.2">
-      <c r="B296" s="8" t="s">
-        <v>238</v>
-      </c>
-      <c r="C296" s="3" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="297" spans="2:9" ht="13.2">
       <c r="B297" s="8" t="s">
         <v>238</v>
       </c>
-      <c r="C297" s="14" t="s">
-        <v>289</v>
+      <c r="C297" s="3" t="s">
+        <v>288</v>
       </c>
     </row>
     <row r="298" spans="2:9" ht="13.2">
       <c r="B298" s="8" t="s">
         <v>238</v>
       </c>
-      <c r="C298" s="3" t="s">
-        <v>290</v>
-      </c>
-      <c r="I298" s="11" t="s">
-        <v>13</v>
+      <c r="C298" s="14" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="299" spans="2:9" ht="13.2">
@@ -4328,7 +4334,10 @@
         <v>238</v>
       </c>
       <c r="C299" s="3" t="s">
-        <v>291</v>
+        <v>290</v>
+      </c>
+      <c r="I299" s="11" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="300" spans="2:9" ht="13.2">
@@ -4336,10 +4345,7 @@
         <v>238</v>
       </c>
       <c r="C300" s="3" t="s">
-        <v>292</v>
-      </c>
-      <c r="H300" s="11" t="s">
-        <v>13</v>
+        <v>291</v>
       </c>
     </row>
     <row r="301" spans="2:9" ht="13.2">
@@ -4347,7 +4353,7 @@
         <v>238</v>
       </c>
       <c r="C301" s="3" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="H301" s="11" t="s">
         <v>13</v>
@@ -4357,8 +4363,8 @@
       <c r="B302" s="8" t="s">
         <v>238</v>
       </c>
-      <c r="C302" s="9" t="s">
-        <v>294</v>
+      <c r="C302" s="3" t="s">
+        <v>293</v>
       </c>
       <c r="H302" s="11" t="s">
         <v>13</v>
@@ -4368,8 +4374,8 @@
       <c r="B303" s="8" t="s">
         <v>238</v>
       </c>
-      <c r="C303" s="3" t="s">
-        <v>295</v>
+      <c r="C303" s="9" t="s">
+        <v>294</v>
       </c>
       <c r="H303" s="11" t="s">
         <v>13</v>
@@ -4380,62 +4386,59 @@
         <v>238</v>
       </c>
       <c r="C304" s="3" t="s">
-        <v>296</v>
+        <v>295</v>
+      </c>
+      <c r="H304" s="11" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="305" spans="2:9" ht="13.2">
       <c r="B305" s="8" t="s">
         <v>238</v>
       </c>
-      <c r="C305" s="9" t="s">
+      <c r="C305" s="3" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="306" spans="2:9" ht="13.2">
+      <c r="B306" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="C306" s="9" t="s">
         <v>297</v>
-      </c>
-    </row>
-    <row r="306" spans="2:9" ht="13.2">
-      <c r="B306" s="6"/>
-      <c r="C306" s="6"/>
-      <c r="I306" s="11" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="307" spans="2:9" ht="13.2">
       <c r="B307" s="6"/>
       <c r="C307" s="6"/>
+      <c r="I307" s="11" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="308" spans="2:9" ht="13.2">
       <c r="B308" s="6"/>
-      <c r="C308" s="25" t="s">
+      <c r="C308" s="6"/>
+    </row>
+    <row r="309" spans="2:9" ht="13.2">
+      <c r="B309" s="6"/>
+      <c r="C309" s="25" t="s">
         <v>298</v>
-      </c>
-    </row>
-    <row r="309" spans="2:9" ht="13.2">
-      <c r="B309" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C309" s="3" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="310" spans="2:9" ht="13.2">
       <c r="B310" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C310" s="9" t="s">
-        <v>300</v>
+      <c r="C310" s="3" t="s">
+        <v>299</v>
       </c>
     </row>
     <row r="311" spans="2:9" ht="13.2">
       <c r="B311" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C311" s="3" t="s">
-        <v>301</v>
-      </c>
-      <c r="D311" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="I311" s="11" t="s">
-        <v>13</v>
+      <c r="C311" s="9" t="s">
+        <v>300</v>
       </c>
     </row>
     <row r="312" spans="2:9" ht="13.2">
@@ -4443,23 +4446,29 @@
         <v>22</v>
       </c>
       <c r="C312" s="3" t="s">
-        <v>302</v>
+        <v>301</v>
+      </c>
+      <c r="D312" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="I312" s="11" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="313" spans="2:9" ht="13.2">
       <c r="B313" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C313" s="9" t="s">
-        <v>303</v>
+      <c r="C313" s="3" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="314" spans="2:9" ht="13.2">
       <c r="B314" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C314" s="3" t="s">
-        <v>304</v>
+      <c r="C314" s="9" t="s">
+        <v>303</v>
       </c>
     </row>
     <row r="315" spans="2:9" ht="13.2">
@@ -4467,10 +4476,7 @@
         <v>22</v>
       </c>
       <c r="C315" s="3" t="s">
-        <v>305</v>
-      </c>
-      <c r="H315" s="11" t="s">
-        <v>13</v>
+        <v>304</v>
       </c>
     </row>
     <row r="316" spans="2:9" ht="13.2">
@@ -4478,18 +4484,18 @@
         <v>22</v>
       </c>
       <c r="C316" s="3" t="s">
-        <v>306</v>
+        <v>305</v>
+      </c>
+      <c r="H316" s="11" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="317" spans="2:9" ht="13.2">
       <c r="B317" s="8" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="C317" s="3" t="s">
-        <v>307</v>
-      </c>
-      <c r="D317" s="11" t="s">
-        <v>13</v>
+        <v>306</v>
       </c>
     </row>
     <row r="318" spans="2:9" ht="13.2">
@@ -4497,9 +4503,9 @@
         <v>38</v>
       </c>
       <c r="C318" s="3" t="s">
-        <v>308</v>
-      </c>
-      <c r="F318" s="11" t="s">
+        <v>307</v>
+      </c>
+      <c r="D318" s="11" t="s">
         <v>13</v>
       </c>
     </row>
@@ -4508,7 +4514,10 @@
         <v>38</v>
       </c>
       <c r="C319" s="3" t="s">
-        <v>309</v>
+        <v>308</v>
+      </c>
+      <c r="F319" s="11" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="320" spans="2:9" ht="13.2">
@@ -4516,38 +4525,35 @@
         <v>38</v>
       </c>
       <c r="C320" s="3" t="s">
-        <v>310</v>
-      </c>
-      <c r="H320" s="11" t="s">
-        <v>13</v>
+        <v>309</v>
       </c>
     </row>
     <row r="321" spans="2:8" ht="13.2">
       <c r="B321" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C321" s="14" t="s">
-        <v>311</v>
-      </c>
-      <c r="H321" s="11"/>
+      <c r="C321" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="H321" s="11" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="322" spans="2:8" ht="13.2">
       <c r="B322" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C322" s="9" t="s">
-        <v>312</v>
-      </c>
-      <c r="H322" s="11" t="s">
-        <v>13</v>
-      </c>
+      <c r="C322" s="14" t="s">
+        <v>311</v>
+      </c>
+      <c r="H322" s="11"/>
     </row>
     <row r="323" spans="2:8" ht="13.2">
       <c r="B323" s="8" t="s">
         <v>38</v>
       </c>
       <c r="C323" s="9" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="H323" s="11" t="s">
         <v>13</v>
@@ -4558,9 +4564,9 @@
         <v>38</v>
       </c>
       <c r="C324" s="9" t="s">
-        <v>314</v>
-      </c>
-      <c r="E324" s="11" t="s">
+        <v>313</v>
+      </c>
+      <c r="H324" s="11" t="s">
         <v>13</v>
       </c>
     </row>
@@ -4569,7 +4575,10 @@
         <v>38</v>
       </c>
       <c r="C325" s="9" t="s">
-        <v>315</v>
+        <v>314</v>
+      </c>
+      <c r="E325" s="11" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="326" spans="2:8" ht="13.2">
@@ -4577,28 +4586,25 @@
         <v>38</v>
       </c>
       <c r="C326" s="9" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="327" spans="2:8" ht="13.2">
+      <c r="B327" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C327" s="9" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="327" spans="2:8" ht="13.2">
-      <c r="B327" s="6"/>
-      <c r="C327" s="6"/>
-    </row>
-    <row r="328" spans="2:8" ht="13.8">
+    <row r="328" spans="2:8" ht="13.2">
       <c r="B328" s="6"/>
-      <c r="C328" s="26" t="s">
+      <c r="C328" s="6"/>
+    </row>
+    <row r="329" spans="2:8" ht="13.8">
+      <c r="B329" s="6"/>
+      <c r="C329" s="26" t="s">
         <v>317</v>
-      </c>
-    </row>
-    <row r="329" spans="2:8" ht="13.2">
-      <c r="B329" s="8" t="s">
-        <v>318</v>
-      </c>
-      <c r="C329" s="9" t="s">
-        <v>319</v>
-      </c>
-      <c r="D329" s="11" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="330" spans="2:8" ht="13.2">
@@ -4606,9 +4612,9 @@
         <v>318</v>
       </c>
       <c r="C330" s="9" t="s">
-        <v>320</v>
-      </c>
-      <c r="G330" s="11" t="s">
+        <v>319</v>
+      </c>
+      <c r="D330" s="11" t="s">
         <v>13</v>
       </c>
     </row>
@@ -4617,7 +4623,10 @@
         <v>318</v>
       </c>
       <c r="C331" s="9" t="s">
-        <v>95</v>
+        <v>320</v>
+      </c>
+      <c r="G331" s="11" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="332" spans="2:8" ht="13.2">
@@ -4625,14 +4634,22 @@
         <v>318</v>
       </c>
       <c r="C332" s="9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="333" spans="2:8" ht="13.2">
+      <c r="B333" s="8" t="s">
+        <v>318</v>
+      </c>
+      <c r="C333" s="9" t="s">
         <v>321</v>
       </c>
-      <c r="H332" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="333" spans="2:8" ht="13.2">
-      <c r="E333" s="11" t="s">
+      <c r="H333" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="334" spans="2:8" ht="13.2">
+      <c r="E334" s="11" t="s">
         <v>13</v>
       </c>
     </row>
@@ -4830,113 +4847,113 @@
     <hyperlink ref="C212" r:id="rId190" xr:uid="{00000000-0004-0000-0000-0000BE000000}"/>
     <hyperlink ref="C213" r:id="rId191" xr:uid="{00000000-0004-0000-0000-0000BF000000}"/>
     <hyperlink ref="C214" r:id="rId192" xr:uid="{00000000-0004-0000-0000-0000C0000000}"/>
-    <hyperlink ref="C215" r:id="rId193" xr:uid="{00000000-0004-0000-0000-0000C1000000}"/>
-    <hyperlink ref="C216" r:id="rId194" xr:uid="{00000000-0004-0000-0000-0000C2000000}"/>
-    <hyperlink ref="C217" r:id="rId195" xr:uid="{00000000-0004-0000-0000-0000C3000000}"/>
-    <hyperlink ref="C218" r:id="rId196" xr:uid="{00000000-0004-0000-0000-0000C4000000}"/>
-    <hyperlink ref="C219" r:id="rId197" xr:uid="{00000000-0004-0000-0000-0000C5000000}"/>
-    <hyperlink ref="C220" r:id="rId198" xr:uid="{00000000-0004-0000-0000-0000C6000000}"/>
-    <hyperlink ref="C221" r:id="rId199" xr:uid="{00000000-0004-0000-0000-0000C7000000}"/>
-    <hyperlink ref="C222" r:id="rId200" xr:uid="{00000000-0004-0000-0000-0000C8000000}"/>
-    <hyperlink ref="C223" r:id="rId201" xr:uid="{00000000-0004-0000-0000-0000C9000000}"/>
-    <hyperlink ref="C224" r:id="rId202" xr:uid="{00000000-0004-0000-0000-0000CA000000}"/>
-    <hyperlink ref="C225" r:id="rId203" xr:uid="{00000000-0004-0000-0000-0000CB000000}"/>
-    <hyperlink ref="C226" r:id="rId204" xr:uid="{00000000-0004-0000-0000-0000CC000000}"/>
-    <hyperlink ref="C227" r:id="rId205" xr:uid="{00000000-0004-0000-0000-0000CD000000}"/>
-    <hyperlink ref="C228" r:id="rId206" xr:uid="{00000000-0004-0000-0000-0000CE000000}"/>
-    <hyperlink ref="C229" r:id="rId207" xr:uid="{00000000-0004-0000-0000-0000CF000000}"/>
-    <hyperlink ref="C230" r:id="rId208" xr:uid="{00000000-0004-0000-0000-0000D0000000}"/>
-    <hyperlink ref="C232" r:id="rId209" xr:uid="{00000000-0004-0000-0000-0000D1000000}"/>
-    <hyperlink ref="C233" r:id="rId210" xr:uid="{00000000-0004-0000-0000-0000D2000000}"/>
-    <hyperlink ref="C234" r:id="rId211" xr:uid="{00000000-0004-0000-0000-0000D3000000}"/>
-    <hyperlink ref="C235" r:id="rId212" xr:uid="{00000000-0004-0000-0000-0000D4000000}"/>
-    <hyperlink ref="C236" r:id="rId213" xr:uid="{00000000-0004-0000-0000-0000D5000000}"/>
-    <hyperlink ref="C237" r:id="rId214" xr:uid="{00000000-0004-0000-0000-0000D6000000}"/>
-    <hyperlink ref="C238" r:id="rId215" xr:uid="{00000000-0004-0000-0000-0000D7000000}"/>
-    <hyperlink ref="C242" r:id="rId216" xr:uid="{00000000-0004-0000-0000-0000D8000000}"/>
-    <hyperlink ref="C243" r:id="rId217" xr:uid="{00000000-0004-0000-0000-0000D9000000}"/>
-    <hyperlink ref="C244" r:id="rId218" xr:uid="{00000000-0004-0000-0000-0000DA000000}"/>
-    <hyperlink ref="C245" r:id="rId219" xr:uid="{00000000-0004-0000-0000-0000DB000000}"/>
-    <hyperlink ref="C246" r:id="rId220" xr:uid="{00000000-0004-0000-0000-0000DC000000}"/>
-    <hyperlink ref="C247" r:id="rId221" xr:uid="{00000000-0004-0000-0000-0000DD000000}"/>
-    <hyperlink ref="C248" r:id="rId222" xr:uid="{00000000-0004-0000-0000-0000DE000000}"/>
-    <hyperlink ref="C249" r:id="rId223" xr:uid="{00000000-0004-0000-0000-0000DF000000}"/>
-    <hyperlink ref="C250" r:id="rId224" xr:uid="{00000000-0004-0000-0000-0000E0000000}"/>
-    <hyperlink ref="C251" r:id="rId225" xr:uid="{00000000-0004-0000-0000-0000E1000000}"/>
-    <hyperlink ref="C252" r:id="rId226" xr:uid="{00000000-0004-0000-0000-0000E2000000}"/>
-    <hyperlink ref="C253" r:id="rId227" xr:uid="{00000000-0004-0000-0000-0000E3000000}"/>
-    <hyperlink ref="C254" r:id="rId228" xr:uid="{00000000-0004-0000-0000-0000E4000000}"/>
-    <hyperlink ref="C255" r:id="rId229" xr:uid="{00000000-0004-0000-0000-0000E5000000}"/>
-    <hyperlink ref="C257" r:id="rId230" xr:uid="{00000000-0004-0000-0000-0000E6000000}"/>
-    <hyperlink ref="C258" r:id="rId231" xr:uid="{00000000-0004-0000-0000-0000E7000000}"/>
-    <hyperlink ref="C259" r:id="rId232" xr:uid="{00000000-0004-0000-0000-0000E8000000}"/>
-    <hyperlink ref="C260" r:id="rId233" xr:uid="{00000000-0004-0000-0000-0000E9000000}"/>
-    <hyperlink ref="C261" r:id="rId234" xr:uid="{00000000-0004-0000-0000-0000EA000000}"/>
-    <hyperlink ref="C262" r:id="rId235" xr:uid="{00000000-0004-0000-0000-0000EB000000}"/>
-    <hyperlink ref="C263" r:id="rId236" xr:uid="{00000000-0004-0000-0000-0000EC000000}"/>
-    <hyperlink ref="C264" r:id="rId237" xr:uid="{00000000-0004-0000-0000-0000ED000000}"/>
-    <hyperlink ref="C265" r:id="rId238" xr:uid="{00000000-0004-0000-0000-0000EE000000}"/>
-    <hyperlink ref="C266" r:id="rId239" xr:uid="{00000000-0004-0000-0000-0000EF000000}"/>
-    <hyperlink ref="C267" r:id="rId240" xr:uid="{00000000-0004-0000-0000-0000F0000000}"/>
-    <hyperlink ref="C268" r:id="rId241" xr:uid="{00000000-0004-0000-0000-0000F1000000}"/>
-    <hyperlink ref="C269" r:id="rId242" xr:uid="{00000000-0004-0000-0000-0000F2000000}"/>
-    <hyperlink ref="C270" r:id="rId243" xr:uid="{00000000-0004-0000-0000-0000F3000000}"/>
-    <hyperlink ref="C271" r:id="rId244" xr:uid="{00000000-0004-0000-0000-0000F4000000}"/>
-    <hyperlink ref="C272" r:id="rId245" xr:uid="{00000000-0004-0000-0000-0000F5000000}"/>
-    <hyperlink ref="C273" r:id="rId246" xr:uid="{00000000-0004-0000-0000-0000F6000000}"/>
-    <hyperlink ref="C274" r:id="rId247" xr:uid="{00000000-0004-0000-0000-0000F7000000}"/>
-    <hyperlink ref="C275" r:id="rId248" xr:uid="{00000000-0004-0000-0000-0000F8000000}"/>
-    <hyperlink ref="C276" r:id="rId249" xr:uid="{00000000-0004-0000-0000-0000F9000000}"/>
-    <hyperlink ref="C277" r:id="rId250" xr:uid="{00000000-0004-0000-0000-0000FA000000}"/>
-    <hyperlink ref="C278" r:id="rId251" xr:uid="{00000000-0004-0000-0000-0000FB000000}"/>
-    <hyperlink ref="C279" r:id="rId252" xr:uid="{00000000-0004-0000-0000-0000FC000000}"/>
-    <hyperlink ref="C280" r:id="rId253" xr:uid="{00000000-0004-0000-0000-0000FD000000}"/>
-    <hyperlink ref="C281" r:id="rId254" xr:uid="{00000000-0004-0000-0000-0000FE000000}"/>
-    <hyperlink ref="C282" r:id="rId255" xr:uid="{00000000-0004-0000-0000-0000FF000000}"/>
-    <hyperlink ref="C283" r:id="rId256" xr:uid="{00000000-0004-0000-0000-000000010000}"/>
-    <hyperlink ref="C284" r:id="rId257" xr:uid="{00000000-0004-0000-0000-000001010000}"/>
-    <hyperlink ref="C285" r:id="rId258" xr:uid="{00000000-0004-0000-0000-000002010000}"/>
-    <hyperlink ref="C286" r:id="rId259" xr:uid="{00000000-0004-0000-0000-000003010000}"/>
-    <hyperlink ref="C287" r:id="rId260" xr:uid="{00000000-0004-0000-0000-000004010000}"/>
-    <hyperlink ref="C289" r:id="rId261" xr:uid="{00000000-0004-0000-0000-000005010000}"/>
-    <hyperlink ref="C290" r:id="rId262" xr:uid="{00000000-0004-0000-0000-000006010000}"/>
-    <hyperlink ref="C291" r:id="rId263" xr:uid="{00000000-0004-0000-0000-000007010000}"/>
-    <hyperlink ref="C292" r:id="rId264" xr:uid="{00000000-0004-0000-0000-000008010000}"/>
-    <hyperlink ref="C295" r:id="rId265" xr:uid="{00000000-0004-0000-0000-000009010000}"/>
-    <hyperlink ref="C296" r:id="rId266" xr:uid="{00000000-0004-0000-0000-00000A010000}"/>
-    <hyperlink ref="C297" r:id="rId267" xr:uid="{00000000-0004-0000-0000-00000B010000}"/>
-    <hyperlink ref="C298" r:id="rId268" xr:uid="{00000000-0004-0000-0000-00000C010000}"/>
-    <hyperlink ref="C299" r:id="rId269" xr:uid="{00000000-0004-0000-0000-00000D010000}"/>
-    <hyperlink ref="C300" r:id="rId270" xr:uid="{00000000-0004-0000-0000-00000E010000}"/>
-    <hyperlink ref="C301" r:id="rId271" xr:uid="{00000000-0004-0000-0000-00000F010000}"/>
-    <hyperlink ref="C302" r:id="rId272" xr:uid="{00000000-0004-0000-0000-000010010000}"/>
-    <hyperlink ref="C303" r:id="rId273" xr:uid="{00000000-0004-0000-0000-000011010000}"/>
-    <hyperlink ref="C304" r:id="rId274" xr:uid="{00000000-0004-0000-0000-000012010000}"/>
-    <hyperlink ref="C305" r:id="rId275" xr:uid="{00000000-0004-0000-0000-000013010000}"/>
-    <hyperlink ref="C308" r:id="rId276" xr:uid="{00000000-0004-0000-0000-000014010000}"/>
-    <hyperlink ref="C309" r:id="rId277" xr:uid="{00000000-0004-0000-0000-000015010000}"/>
-    <hyperlink ref="C310" r:id="rId278" xr:uid="{00000000-0004-0000-0000-000016010000}"/>
-    <hyperlink ref="C311" r:id="rId279" xr:uid="{00000000-0004-0000-0000-000017010000}"/>
-    <hyperlink ref="C312" r:id="rId280" xr:uid="{00000000-0004-0000-0000-000018010000}"/>
-    <hyperlink ref="C313" r:id="rId281" xr:uid="{00000000-0004-0000-0000-000019010000}"/>
-    <hyperlink ref="C314" r:id="rId282" xr:uid="{00000000-0004-0000-0000-00001A010000}"/>
-    <hyperlink ref="C315" r:id="rId283" xr:uid="{00000000-0004-0000-0000-00001B010000}"/>
-    <hyperlink ref="C316" r:id="rId284" xr:uid="{00000000-0004-0000-0000-00001C010000}"/>
-    <hyperlink ref="C317" r:id="rId285" xr:uid="{00000000-0004-0000-0000-00001D010000}"/>
-    <hyperlink ref="C318" r:id="rId286" xr:uid="{00000000-0004-0000-0000-00001E010000}"/>
-    <hyperlink ref="C319" r:id="rId287" xr:uid="{00000000-0004-0000-0000-00001F010000}"/>
-    <hyperlink ref="C320" r:id="rId288" xr:uid="{00000000-0004-0000-0000-000020010000}"/>
-    <hyperlink ref="C321" r:id="rId289" xr:uid="{00000000-0004-0000-0000-000021010000}"/>
-    <hyperlink ref="C322" r:id="rId290" xr:uid="{00000000-0004-0000-0000-000022010000}"/>
-    <hyperlink ref="C323" r:id="rId291" xr:uid="{00000000-0004-0000-0000-000023010000}"/>
-    <hyperlink ref="C324" r:id="rId292" xr:uid="{00000000-0004-0000-0000-000024010000}"/>
-    <hyperlink ref="C325" r:id="rId293" xr:uid="{00000000-0004-0000-0000-000025010000}"/>
-    <hyperlink ref="C326" r:id="rId294" xr:uid="{00000000-0004-0000-0000-000026010000}"/>
-    <hyperlink ref="C328" r:id="rId295" xr:uid="{00000000-0004-0000-0000-000027010000}"/>
-    <hyperlink ref="C329" r:id="rId296" xr:uid="{00000000-0004-0000-0000-000028010000}"/>
-    <hyperlink ref="C330" r:id="rId297" xr:uid="{00000000-0004-0000-0000-000029010000}"/>
-    <hyperlink ref="C331" r:id="rId298" xr:uid="{00000000-0004-0000-0000-00002A010000}"/>
-    <hyperlink ref="C332" r:id="rId299" xr:uid="{00000000-0004-0000-0000-00002B010000}"/>
+    <hyperlink ref="C216" r:id="rId193" xr:uid="{00000000-0004-0000-0000-0000C1000000}"/>
+    <hyperlink ref="C217" r:id="rId194" xr:uid="{00000000-0004-0000-0000-0000C2000000}"/>
+    <hyperlink ref="C218" r:id="rId195" xr:uid="{00000000-0004-0000-0000-0000C3000000}"/>
+    <hyperlink ref="C219" r:id="rId196" xr:uid="{00000000-0004-0000-0000-0000C4000000}"/>
+    <hyperlink ref="C220" r:id="rId197" xr:uid="{00000000-0004-0000-0000-0000C5000000}"/>
+    <hyperlink ref="C221" r:id="rId198" xr:uid="{00000000-0004-0000-0000-0000C6000000}"/>
+    <hyperlink ref="C222" r:id="rId199" xr:uid="{00000000-0004-0000-0000-0000C7000000}"/>
+    <hyperlink ref="C223" r:id="rId200" xr:uid="{00000000-0004-0000-0000-0000C8000000}"/>
+    <hyperlink ref="C224" r:id="rId201" xr:uid="{00000000-0004-0000-0000-0000C9000000}"/>
+    <hyperlink ref="C225" r:id="rId202" xr:uid="{00000000-0004-0000-0000-0000CA000000}"/>
+    <hyperlink ref="C226" r:id="rId203" xr:uid="{00000000-0004-0000-0000-0000CB000000}"/>
+    <hyperlink ref="C227" r:id="rId204" xr:uid="{00000000-0004-0000-0000-0000CC000000}"/>
+    <hyperlink ref="C228" r:id="rId205" xr:uid="{00000000-0004-0000-0000-0000CD000000}"/>
+    <hyperlink ref="C229" r:id="rId206" xr:uid="{00000000-0004-0000-0000-0000CE000000}"/>
+    <hyperlink ref="C230" r:id="rId207" xr:uid="{00000000-0004-0000-0000-0000CF000000}"/>
+    <hyperlink ref="C231" r:id="rId208" xr:uid="{00000000-0004-0000-0000-0000D0000000}"/>
+    <hyperlink ref="C233" r:id="rId209" xr:uid="{00000000-0004-0000-0000-0000D1000000}"/>
+    <hyperlink ref="C234" r:id="rId210" xr:uid="{00000000-0004-0000-0000-0000D2000000}"/>
+    <hyperlink ref="C235" r:id="rId211" xr:uid="{00000000-0004-0000-0000-0000D3000000}"/>
+    <hyperlink ref="C236" r:id="rId212" xr:uid="{00000000-0004-0000-0000-0000D4000000}"/>
+    <hyperlink ref="C237" r:id="rId213" xr:uid="{00000000-0004-0000-0000-0000D5000000}"/>
+    <hyperlink ref="C238" r:id="rId214" xr:uid="{00000000-0004-0000-0000-0000D6000000}"/>
+    <hyperlink ref="C239" r:id="rId215" xr:uid="{00000000-0004-0000-0000-0000D7000000}"/>
+    <hyperlink ref="C243" r:id="rId216" xr:uid="{00000000-0004-0000-0000-0000D8000000}"/>
+    <hyperlink ref="C244" r:id="rId217" xr:uid="{00000000-0004-0000-0000-0000D9000000}"/>
+    <hyperlink ref="C245" r:id="rId218" xr:uid="{00000000-0004-0000-0000-0000DA000000}"/>
+    <hyperlink ref="C246" r:id="rId219" xr:uid="{00000000-0004-0000-0000-0000DB000000}"/>
+    <hyperlink ref="C247" r:id="rId220" xr:uid="{00000000-0004-0000-0000-0000DC000000}"/>
+    <hyperlink ref="C248" r:id="rId221" xr:uid="{00000000-0004-0000-0000-0000DD000000}"/>
+    <hyperlink ref="C249" r:id="rId222" xr:uid="{00000000-0004-0000-0000-0000DE000000}"/>
+    <hyperlink ref="C250" r:id="rId223" xr:uid="{00000000-0004-0000-0000-0000DF000000}"/>
+    <hyperlink ref="C251" r:id="rId224" xr:uid="{00000000-0004-0000-0000-0000E0000000}"/>
+    <hyperlink ref="C252" r:id="rId225" xr:uid="{00000000-0004-0000-0000-0000E1000000}"/>
+    <hyperlink ref="C253" r:id="rId226" xr:uid="{00000000-0004-0000-0000-0000E2000000}"/>
+    <hyperlink ref="C254" r:id="rId227" xr:uid="{00000000-0004-0000-0000-0000E3000000}"/>
+    <hyperlink ref="C255" r:id="rId228" xr:uid="{00000000-0004-0000-0000-0000E4000000}"/>
+    <hyperlink ref="C256" r:id="rId229" xr:uid="{00000000-0004-0000-0000-0000E5000000}"/>
+    <hyperlink ref="C258" r:id="rId230" xr:uid="{00000000-0004-0000-0000-0000E6000000}"/>
+    <hyperlink ref="C259" r:id="rId231" xr:uid="{00000000-0004-0000-0000-0000E7000000}"/>
+    <hyperlink ref="C260" r:id="rId232" xr:uid="{00000000-0004-0000-0000-0000E8000000}"/>
+    <hyperlink ref="C261" r:id="rId233" xr:uid="{00000000-0004-0000-0000-0000E9000000}"/>
+    <hyperlink ref="C262" r:id="rId234" xr:uid="{00000000-0004-0000-0000-0000EA000000}"/>
+    <hyperlink ref="C263" r:id="rId235" xr:uid="{00000000-0004-0000-0000-0000EB000000}"/>
+    <hyperlink ref="C264" r:id="rId236" xr:uid="{00000000-0004-0000-0000-0000EC000000}"/>
+    <hyperlink ref="C265" r:id="rId237" xr:uid="{00000000-0004-0000-0000-0000ED000000}"/>
+    <hyperlink ref="C266" r:id="rId238" xr:uid="{00000000-0004-0000-0000-0000EE000000}"/>
+    <hyperlink ref="C267" r:id="rId239" xr:uid="{00000000-0004-0000-0000-0000EF000000}"/>
+    <hyperlink ref="C268" r:id="rId240" xr:uid="{00000000-0004-0000-0000-0000F0000000}"/>
+    <hyperlink ref="C269" r:id="rId241" xr:uid="{00000000-0004-0000-0000-0000F1000000}"/>
+    <hyperlink ref="C270" r:id="rId242" xr:uid="{00000000-0004-0000-0000-0000F2000000}"/>
+    <hyperlink ref="C271" r:id="rId243" xr:uid="{00000000-0004-0000-0000-0000F3000000}"/>
+    <hyperlink ref="C272" r:id="rId244" xr:uid="{00000000-0004-0000-0000-0000F4000000}"/>
+    <hyperlink ref="C273" r:id="rId245" xr:uid="{00000000-0004-0000-0000-0000F5000000}"/>
+    <hyperlink ref="C274" r:id="rId246" xr:uid="{00000000-0004-0000-0000-0000F6000000}"/>
+    <hyperlink ref="C275" r:id="rId247" xr:uid="{00000000-0004-0000-0000-0000F7000000}"/>
+    <hyperlink ref="C276" r:id="rId248" xr:uid="{00000000-0004-0000-0000-0000F8000000}"/>
+    <hyperlink ref="C277" r:id="rId249" xr:uid="{00000000-0004-0000-0000-0000F9000000}"/>
+    <hyperlink ref="C278" r:id="rId250" xr:uid="{00000000-0004-0000-0000-0000FA000000}"/>
+    <hyperlink ref="C279" r:id="rId251" xr:uid="{00000000-0004-0000-0000-0000FB000000}"/>
+    <hyperlink ref="C280" r:id="rId252" xr:uid="{00000000-0004-0000-0000-0000FC000000}"/>
+    <hyperlink ref="C281" r:id="rId253" xr:uid="{00000000-0004-0000-0000-0000FD000000}"/>
+    <hyperlink ref="C282" r:id="rId254" xr:uid="{00000000-0004-0000-0000-0000FE000000}"/>
+    <hyperlink ref="C283" r:id="rId255" xr:uid="{00000000-0004-0000-0000-0000FF000000}"/>
+    <hyperlink ref="C284" r:id="rId256" xr:uid="{00000000-0004-0000-0000-000000010000}"/>
+    <hyperlink ref="C285" r:id="rId257" xr:uid="{00000000-0004-0000-0000-000001010000}"/>
+    <hyperlink ref="C286" r:id="rId258" xr:uid="{00000000-0004-0000-0000-000002010000}"/>
+    <hyperlink ref="C287" r:id="rId259" xr:uid="{00000000-0004-0000-0000-000003010000}"/>
+    <hyperlink ref="C288" r:id="rId260" xr:uid="{00000000-0004-0000-0000-000004010000}"/>
+    <hyperlink ref="C290" r:id="rId261" xr:uid="{00000000-0004-0000-0000-000005010000}"/>
+    <hyperlink ref="C291" r:id="rId262" xr:uid="{00000000-0004-0000-0000-000006010000}"/>
+    <hyperlink ref="C292" r:id="rId263" xr:uid="{00000000-0004-0000-0000-000007010000}"/>
+    <hyperlink ref="C293" r:id="rId264" xr:uid="{00000000-0004-0000-0000-000008010000}"/>
+    <hyperlink ref="C296" r:id="rId265" xr:uid="{00000000-0004-0000-0000-000009010000}"/>
+    <hyperlink ref="C297" r:id="rId266" xr:uid="{00000000-0004-0000-0000-00000A010000}"/>
+    <hyperlink ref="C298" r:id="rId267" xr:uid="{00000000-0004-0000-0000-00000B010000}"/>
+    <hyperlink ref="C299" r:id="rId268" xr:uid="{00000000-0004-0000-0000-00000C010000}"/>
+    <hyperlink ref="C300" r:id="rId269" xr:uid="{00000000-0004-0000-0000-00000D010000}"/>
+    <hyperlink ref="C301" r:id="rId270" xr:uid="{00000000-0004-0000-0000-00000E010000}"/>
+    <hyperlink ref="C302" r:id="rId271" xr:uid="{00000000-0004-0000-0000-00000F010000}"/>
+    <hyperlink ref="C303" r:id="rId272" xr:uid="{00000000-0004-0000-0000-000010010000}"/>
+    <hyperlink ref="C304" r:id="rId273" xr:uid="{00000000-0004-0000-0000-000011010000}"/>
+    <hyperlink ref="C305" r:id="rId274" xr:uid="{00000000-0004-0000-0000-000012010000}"/>
+    <hyperlink ref="C306" r:id="rId275" xr:uid="{00000000-0004-0000-0000-000013010000}"/>
+    <hyperlink ref="C309" r:id="rId276" xr:uid="{00000000-0004-0000-0000-000014010000}"/>
+    <hyperlink ref="C310" r:id="rId277" xr:uid="{00000000-0004-0000-0000-000015010000}"/>
+    <hyperlink ref="C311" r:id="rId278" xr:uid="{00000000-0004-0000-0000-000016010000}"/>
+    <hyperlink ref="C312" r:id="rId279" xr:uid="{00000000-0004-0000-0000-000017010000}"/>
+    <hyperlink ref="C313" r:id="rId280" xr:uid="{00000000-0004-0000-0000-000018010000}"/>
+    <hyperlink ref="C314" r:id="rId281" xr:uid="{00000000-0004-0000-0000-000019010000}"/>
+    <hyperlink ref="C315" r:id="rId282" xr:uid="{00000000-0004-0000-0000-00001A010000}"/>
+    <hyperlink ref="C316" r:id="rId283" xr:uid="{00000000-0004-0000-0000-00001B010000}"/>
+    <hyperlink ref="C317" r:id="rId284" xr:uid="{00000000-0004-0000-0000-00001C010000}"/>
+    <hyperlink ref="C318" r:id="rId285" xr:uid="{00000000-0004-0000-0000-00001D010000}"/>
+    <hyperlink ref="C319" r:id="rId286" xr:uid="{00000000-0004-0000-0000-00001E010000}"/>
+    <hyperlink ref="C320" r:id="rId287" xr:uid="{00000000-0004-0000-0000-00001F010000}"/>
+    <hyperlink ref="C321" r:id="rId288" xr:uid="{00000000-0004-0000-0000-000020010000}"/>
+    <hyperlink ref="C322" r:id="rId289" xr:uid="{00000000-0004-0000-0000-000021010000}"/>
+    <hyperlink ref="C323" r:id="rId290" xr:uid="{00000000-0004-0000-0000-000022010000}"/>
+    <hyperlink ref="C324" r:id="rId291" xr:uid="{00000000-0004-0000-0000-000023010000}"/>
+    <hyperlink ref="C325" r:id="rId292" xr:uid="{00000000-0004-0000-0000-000024010000}"/>
+    <hyperlink ref="C326" r:id="rId293" xr:uid="{00000000-0004-0000-0000-000025010000}"/>
+    <hyperlink ref="C327" r:id="rId294" xr:uid="{00000000-0004-0000-0000-000026010000}"/>
+    <hyperlink ref="C329" r:id="rId295" xr:uid="{00000000-0004-0000-0000-000027010000}"/>
+    <hyperlink ref="C330" r:id="rId296" xr:uid="{00000000-0004-0000-0000-000028010000}"/>
+    <hyperlink ref="C331" r:id="rId297" xr:uid="{00000000-0004-0000-0000-000029010000}"/>
+    <hyperlink ref="C332" r:id="rId298" xr:uid="{00000000-0004-0000-0000-00002A010000}"/>
+    <hyperlink ref="C333" r:id="rId299" xr:uid="{00000000-0004-0000-0000-00002B010000}"/>
     <hyperlink ref="C133" r:id="rId300" xr:uid="{00000000-0004-0000-0000-000073000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Stack and Queues/Graph: (24)Rotten Oranges.cpp
</commit_message>
<xml_diff>
--- a/#DSASheetbyArsh (45-60 Days).xlsx
+++ b/#DSASheetbyArsh (45-60 Days).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kunal\OneDrive\Desktop\vs code\45DaysDSAChallenge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42A5E9CC-8068-490B-A8C3-B4F92A366EC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DB600FE-0F7F-4C9E-B6C5-91CC754B06A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="812" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="813" uniqueCount="332">
   <si>
     <t>#CrackYourInternship</t>
   </si>
@@ -1045,6 +1045,9 @@
   </si>
   <si>
     <t>Done(11/07/23)</t>
+  </si>
+  <si>
+    <t>Done(17/07/23</t>
   </si>
 </sst>
 </file>
@@ -1512,8 +1515,8 @@
   </sheetPr>
   <dimension ref="A1:I334"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B192" zoomScale="87" workbookViewId="0">
-      <selection activeCell="D196" sqref="D196"/>
+    <sheetView tabSelected="1" topLeftCell="B124" zoomScale="87" workbookViewId="0">
+      <selection activeCell="E137" sqref="E137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -2776,6 +2779,9 @@
       </c>
       <c r="C134" s="9" t="s">
         <v>134</v>
+      </c>
+      <c r="D134" t="s">
+        <v>331</v>
       </c>
       <c r="G134" s="11" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Graph: (25)Detect Cycle in Undirected Graph.cpp
</commit_message>
<xml_diff>
--- a/#DSASheetbyArsh (45-60 Days).xlsx
+++ b/#DSASheetbyArsh (45-60 Days).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kunal\OneDrive\Desktop\vs code\45DaysDSAChallenge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DB600FE-0F7F-4C9E-B6C5-91CC754B06A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE3A384E-61A0-4F36-98F8-ECD5C21B0FF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="813" uniqueCount="332">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="814" uniqueCount="333">
   <si>
     <t>#CrackYourInternship</t>
   </si>
@@ -1048,6 +1048,9 @@
   </si>
   <si>
     <t>Done(17/07/23</t>
+  </si>
+  <si>
+    <t>Done(17/07/23)</t>
   </si>
 </sst>
 </file>
@@ -1515,8 +1518,8 @@
   </sheetPr>
   <dimension ref="A1:I334"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B124" zoomScale="87" workbookViewId="0">
-      <selection activeCell="E137" sqref="E137"/>
+    <sheetView tabSelected="1" topLeftCell="B187" zoomScale="87" workbookViewId="0">
+      <selection activeCell="C200" sqref="C200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -3438,6 +3441,9 @@
       </c>
       <c r="C199" s="9" t="s">
         <v>197</v>
+      </c>
+      <c r="D199" t="s">
+        <v>332</v>
       </c>
     </row>
     <row r="200" spans="2:7" ht="13.2">

</xml_diff>

<commit_message>
Matrix/Graph: (26)No. of Islands.cpp
</commit_message>
<xml_diff>
--- a/#DSASheetbyArsh (45-60 Days).xlsx
+++ b/#DSASheetbyArsh (45-60 Days).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kunal\OneDrive\Desktop\vs code\45DaysDSAChallenge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE3A384E-61A0-4F36-98F8-ECD5C21B0FF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{531ABB47-91B4-4FBE-82E7-E1B592976EA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="814" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="815" uniqueCount="333">
   <si>
     <t>#CrackYourInternship</t>
   </si>
@@ -1518,8 +1518,8 @@
   </sheetPr>
   <dimension ref="A1:I334"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B187" zoomScale="87" workbookViewId="0">
-      <selection activeCell="C200" sqref="C200"/>
+    <sheetView tabSelected="1" topLeftCell="B50" zoomScale="87" workbookViewId="0">
+      <selection activeCell="E60" sqref="E60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -2101,6 +2101,9 @@
       </c>
       <c r="C60" s="9" t="s">
         <v>66</v>
+      </c>
+      <c r="D60" t="s">
+        <v>332</v>
       </c>
     </row>
     <row r="61" spans="2:8" ht="13.2">

</xml_diff>

<commit_message>
Stack and Queues/Graph/Matrix: (28)Distance of nearest cell having 1
</commit_message>
<xml_diff>
--- a/#DSASheetbyArsh (45-60 Days).xlsx
+++ b/#DSASheetbyArsh (45-60 Days).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kunal\OneDrive\Desktop\vs code\45DaysDSAChallenge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{531ABB47-91B4-4FBE-82E7-E1B592976EA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75DFF3A6-708F-4738-BFDA-6B7162B06618}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="815" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="817" uniqueCount="334">
   <si>
     <t>#CrackYourInternship</t>
   </si>
@@ -1051,6 +1051,9 @@
   </si>
   <si>
     <t>Done(17/07/23)</t>
+  </si>
+  <si>
+    <t>Done(18/07/23)</t>
   </si>
 </sst>
 </file>
@@ -1518,8 +1521,8 @@
   </sheetPr>
   <dimension ref="A1:I334"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B50" zoomScale="87" workbookViewId="0">
-      <selection activeCell="E60" sqref="E60"/>
+    <sheetView tabSelected="1" topLeftCell="B124" zoomScale="87" workbookViewId="0">
+      <selection activeCell="F131" sqref="F131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -2761,6 +2764,9 @@
       <c r="C132" s="14" t="s">
         <v>132</v>
       </c>
+      <c r="D132" t="s">
+        <v>333</v>
+      </c>
       <c r="I132" s="11" t="s">
         <v>13</v>
       </c>
@@ -3414,6 +3420,9 @@
       </c>
       <c r="C196" s="9" t="s">
         <v>194</v>
+      </c>
+      <c r="D196" t="s">
+        <v>332</v>
       </c>
     </row>
     <row r="197" spans="2:7" ht="13.2">

</xml_diff>

<commit_message>
Array: (29)Best Time to Buy and Sell Stock.cpp
</commit_message>
<xml_diff>
--- a/#DSASheetbyArsh (45-60 Days).xlsx
+++ b/#DSASheetbyArsh (45-60 Days).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kunal\OneDrive\Desktop\vs code\45DaysDSAChallenge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75DFF3A6-708F-4738-BFDA-6B7162B06618}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1BBCC17-315C-437B-82A6-5488FF162C68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7740" yWindow="2472" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="817" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="818" uniqueCount="334">
   <si>
     <t>#CrackYourInternship</t>
   </si>
@@ -1521,8 +1521,8 @@
   </sheetPr>
   <dimension ref="A1:I334"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B124" zoomScale="87" workbookViewId="0">
-      <selection activeCell="F131" sqref="F131"/>
+    <sheetView tabSelected="1" zoomScale="87" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -1572,9 +1572,6 @@
       <c r="C5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D5" t="s">
-        <v>322</v>
-      </c>
     </row>
     <row r="6" spans="1:9" ht="13.2">
       <c r="B6" s="8" t="s">
@@ -1597,6 +1594,9 @@
       <c r="C7" s="9" t="s">
         <v>14</v>
       </c>
+      <c r="D7" t="s">
+        <v>322</v>
+      </c>
       <c r="E7" s="10" t="s">
         <v>13</v>
       </c>
@@ -1613,6 +1613,9 @@
       </c>
       <c r="C8" s="9" t="s">
         <v>15</v>
+      </c>
+      <c r="D8" t="s">
+        <v>333</v>
       </c>
       <c r="E8" s="10" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Tree: (87) Max Path Sum.cpp
</commit_message>
<xml_diff>
--- a/#DSASheetbyArsh (45-60 Days).xlsx
+++ b/#DSASheetbyArsh (45-60 Days).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kunal\OneDrive\Desktop\vs code\45DaysDSAChallenge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C5A8364-EE37-4D7D-B5F4-5C72C607D6ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA3CC0E8-32AB-4282-A553-D43D23C4439E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1272" yWindow="1548" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="824" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="827" uniqueCount="338">
   <si>
     <t>#CrackYourInternship</t>
   </si>
@@ -1533,8 +1533,8 @@
   </sheetPr>
   <dimension ref="A1:I334"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" zoomScale="80" workbookViewId="0">
-      <selection activeCell="C68" sqref="C68"/>
+    <sheetView tabSelected="1" topLeftCell="A277" zoomScale="80" workbookViewId="0">
+      <selection activeCell="D291" sqref="D291"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -1741,6 +1741,9 @@
       <c r="C18" s="9" t="s">
         <v>26</v>
       </c>
+      <c r="D18" t="s">
+        <v>336</v>
+      </c>
       <c r="E18" s="10" t="s">
         <v>13</v>
       </c>
@@ -1752,6 +1755,9 @@
       </c>
       <c r="C19" s="9" t="s">
         <v>27</v>
+      </c>
+      <c r="D19" t="s">
+        <v>336</v>
       </c>
       <c r="F19" s="10" t="s">
         <v>13</v>
@@ -4335,6 +4341,9 @@
       </c>
       <c r="C291" s="3" t="s">
         <v>18</v>
+      </c>
+      <c r="D291" t="s">
+        <v>336</v>
       </c>
       <c r="H291" s="11" t="s">
         <v>13</v>

</xml_diff>